<commit_message>
Issue SEO-1, SEO-2 and SEO-3 in SEO Template implemented.
</commit_message>
<xml_diff>
--- a/Template-SEO-audit.xlsx
+++ b/Template-SEO-audit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicopatsch/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="304" documentId="11_05D6EA6CE7DA307BAFC13D42CE951501BDC39C52" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E82A5668-4105-45EA-A932-4EFCE143D87F}"/>
+  <xr:revisionPtr revIDLastSave="434" documentId="11_05D6EA6CE7DA307BAFC13D42CE951501BDC39C52" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{691B2F65-EBC8-47DC-AB28-15FFCC8C5525}"/>
   <bookViews>
     <workbookView xWindow="940" yWindow="460" windowWidth="27860" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="89">
   <si>
     <t>Category</t>
   </si>
@@ -62,7 +62,7 @@
     <t>Reference</t>
   </si>
   <si>
-    <t>Accessibility</t>
+    <t>Accessibility-1</t>
   </si>
   <si>
     <t>lang attribute value is invalid. "&lt;html lang="Default"&gt;"</t>
@@ -80,6 +80,9 @@
     <t>https://www.w3.org/WAI/WCAG21/quickref/?showtechniques=311#language-of-page</t>
   </si>
   <si>
+    <t>Accessibility-2</t>
+  </si>
+  <si>
     <t>The page title is missing or not descriptive.</t>
   </si>
   <si>
@@ -89,36 +92,16 @@
     <t>Add titles to web pages that describe topic or purpose.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>Change code to something like:
-    &lt;title&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>Freelance Web Design Services by Mike in Atlanta</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>&lt;/title&gt;</t>
-    </r>
+    <t>Change code to something like:
+    &lt;title&gt;Freelance Web Design Services by Mike in Atlanta&lt;/title&gt;</t>
   </si>
   <si>
     <t>https://webaim.org/standards/wcag/checklist#sc2.4.2</t>
   </si>
   <si>
+    <t>Accessibility-3</t>
+  </si>
+  <si>
     <t>Line 239: Alternative text is insufficient</t>
   </si>
   <si>
@@ -132,6 +115,9 @@
   </si>
   <si>
     <t>https://webaim.org/standards/wcag/checklist#sc1.1.1</t>
+  </si>
+  <si>
+    <t>Accessibility-4</t>
   </si>
   <si>
     <t>Page 2,Line 103: A &lt;label&gt; element missing a for attribute value that is equal to the id of a unique form control.</t>
@@ -174,6 +160,9 @@
     <t>&lt;- Form inputs have associated text labels.</t>
   </si>
   <si>
+    <t>Accessibility-5</t>
+  </si>
+  <si>
     <t xml:space="preserve">Page 2,Line 102: Grouping method are insufficient for accessibility. </t>
   </si>
   <si>
@@ -191,6 +180,9 @@
   <si>
     <t>&lt;- Situation A: H71
 &lt;- Replicate the OC example with fieldset</t>
+  </si>
+  <si>
+    <t>Accessibility-6</t>
   </si>
   <si>
     <t>Line 351: An anchor element has an href attribute, but contains no text (or only spaces) and no images with alternative text.</t>
@@ -249,6 +241,9 @@
     <t>https://www.w3.org/WAI/WCAG21/quickref/?showtechniques=244#link-purpose-in-context</t>
   </si>
   <si>
+    <t>Accessibility-7</t>
+  </si>
+  <si>
     <t>Line 122,171: If the same visual presentation can be made using text alone, an image is not used to present that text.</t>
   </si>
   <si>
@@ -259,12 +254,15 @@
 C30: Using CSS to replace text with images of text and providing user interface controls to switch</t>
   </si>
   <si>
-    <t>Replace the img with html content, and style it similarly as in the img. Or at least change the alt text to match the text in the img file.</t>
+    <t>Replace the img with html content, and style it similarly as in the img. Or(altough I don't recommend it) at least change the alt text to match the text in the img file.</t>
   </si>
   <si>
     <t>https://www.w3.org/WAI/WCAG21/quickref/?showtechniques=244%2C145#images-of-text</t>
   </si>
   <si>
+    <t>Accessibility-8</t>
+  </si>
+  <si>
     <t>Line 101: Very low contrast between text and background colors.</t>
   </si>
   <si>
@@ -283,6 +281,9 @@
     <t>&lt;- Situation B:G145</t>
   </si>
   <si>
+    <t>Accessibility-9</t>
+  </si>
+  <si>
     <t xml:space="preserve">Page2: The link/logo(which was present on the home page nav bar) that leads back to the main page is unclicable.  </t>
   </si>
   <si>
@@ -301,10 +302,132 @@
     <t>Maybe this is not an accessability issue. As I could found it with TAB key. But it's an issue</t>
   </si>
   <si>
+    <t>Accessibility-10</t>
+  </si>
+  <si>
     <t>F63: Failure of Success Criterion 2.4.4 due to providing link context only in content that is not related to the link</t>
   </si>
   <si>
-    <t>(SEO or Accessibility?)</t>
+    <t>SEO-1</t>
+  </si>
+  <si>
+    <t>Line 122, issue-1: Image element was used instead of H1 element for the "main title"/theme of the page.</t>
+  </si>
+  <si>
+    <t>The h1 element helps defining the main content/keywords regards what the page is all about to search engines.(Similarly to the title tag, but there is some differences)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Include the exact keywords in your h1 element you have in your tilte tag and use exact match or replaced with a synonym in h2 tags.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">&lt;title&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Websites and graphic design</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> - GoMike Designs &lt;/title&gt;
+&lt;h1&gt; I create </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>websites and graphic design</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> that help Atlanta companies become attractive and recognizable online. &lt;/h1&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>SEO-2</t>
+  </si>
+  <si>
+    <t>Line 122, issue-2:Responsiveness was not set for this element.</t>
+  </si>
+  <si>
+    <t>Google now uses the mobile version of your site (if it exists) as the primary version for indexing purposes. The better the mobile version of your site performs, the more likely will appear higher in search results. So if you don't have a mobile verision responsivness is a must for SEO.</t>
+  </si>
+  <si>
+    <t>If you have the budget make a mobile version of your site.If not, it's ok just code your webpages mobile-first, than adapt to tablet and desktop. Google will appreciate this and get you higher in his search results.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Change the img tag to an h1 and hardcode the text:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>&lt;h1&gt; I create websites and design graphics that help Atlanta companies become attractive and recognizable online. &lt;/h1&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>https://developers.google.com/search/mobile-sites/mobile-first-indexing</t>
+  </si>
+  <si>
+    <t>SEO-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Missing good sematic stracture.(mostly just dives, instead of header,main, footer etc.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Semantic tags makes web pages more informative and adaptable, allowing browsers and search engines to better interpret content. </t>
+  </si>
+  <si>
+    <t>Use semantic tags whenever it's possible.</t>
+  </si>
+  <si>
+    <t>For example: Add Header, main, section and footer semantic tags (Check amended code).</t>
+  </si>
+  <si>
+    <t>SEO-4</t>
+  </si>
+  <si>
+    <t>Line 44: Putting keywords in a hidden div. This considered "black hat" technique</t>
+  </si>
+  <si>
+    <t>I strongly advise against using black hat SEO techniques on an established company’s website. You run the risk of having your website excluded from Google search results.</t>
+  </si>
+  <si>
+    <t>Place your keywords in your title tag, description, h1,h2...etc. elements, paragraphs and image alt attribute, in a way it's also natural for the reader. (Otherwise its "keyword stuffing" and is considered a black hat technique as well.)</t>
+  </si>
+  <si>
+    <t>Remove divs with keywords classes.</t>
+  </si>
+  <si>
+    <t>SEO-5</t>
   </si>
   <si>
     <t>Supplimentary info:</t>
@@ -420,7 +543,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -453,6 +576,10 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -669,10 +796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -749,260 +876,310 @@
     </row>
     <row r="3" spans="1:26" ht="162">
       <c r="A3" s="6" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="6" t="s">
         <v>15</v>
       </c>
+      <c r="E3" s="11" t="s">
+        <v>16</v>
+      </c>
       <c r="F3" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:26" ht="275.25">
       <c r="A4" s="6" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:26" ht="113.25">
       <c r="A5" s="6" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="G5" s="6" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="146.25">
       <c r="A6" s="6" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="162">
       <c r="A7" s="6" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:26" ht="259.5">
       <c r="A8" s="6" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:26" ht="64.5">
       <c r="A9" s="6" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="146.25">
       <c r="A10" s="6" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="64.5">
       <c r="A11" s="6" t="s">
-        <v>6</v>
+        <v>63</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:26" ht="32.25">
+    <row r="12" spans="1:26" ht="201.75" customHeight="1">
       <c r="A12" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
+        <v>65</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:26" ht="32.25">
+    <row r="13" spans="1:26" ht="194.25">
       <c r="A13" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
+        <v>70</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>75</v>
+      </c>
     </row>
-    <row r="14" spans="1:26" ht="32.25">
+    <row r="14" spans="1:26" ht="96.75">
       <c r="A14" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
+        <v>76</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:26" ht="32.25">
-      <c r="A15" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
+    <row r="15" spans="1:26" s="13" customFormat="1" ht="146.25">
+      <c r="A15" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>85</v>
+      </c>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:26" ht="113.25">
-      <c r="A16" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>58</v>
-      </c>
+    <row r="16" spans="1:26" ht="15.75">
+      <c r="A16" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" ht="15.75" customHeight="1"/>
-    <row r="18" ht="15.75" customHeight="1"/>
-    <row r="19" ht="15.75" customHeight="1"/>
-    <row r="20" ht="15.75" customHeight="1"/>
-    <row r="21" ht="15.75" customHeight="1"/>
-    <row r="22" ht="15.75" customHeight="1"/>
-    <row r="23" ht="15.75" customHeight="1"/>
-    <row r="24" ht="15.75" customHeight="1"/>
-    <row r="25" ht="15.75" customHeight="1"/>
-    <row r="26" ht="15.75" customHeight="1"/>
-    <row r="27" ht="15.75" customHeight="1"/>
-    <row r="28" ht="15.75" customHeight="1"/>
-    <row r="29" ht="15.75" customHeight="1"/>
-    <row r="30" ht="15.75" customHeight="1"/>
-    <row r="31" ht="15.75" customHeight="1"/>
-    <row r="32" ht="15.75" customHeight="1"/>
+    <row r="17" spans="1:6" ht="15.75">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="19" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="20" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="22" spans="1:6" ht="113.25">
+      <c r="A22" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="27" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="30" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="31" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="32" spans="1:6" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
@@ -1971,6 +2148,7 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" location="language-of-page" xr:uid="{BDC05546-EDF3-4630-92C7-EE1076FF788B}"/>
@@ -1982,6 +2160,7 @@
     <hyperlink ref="F3" r:id="rId7" location="sc2.4.2" xr:uid="{B37EBE60-CB4A-4274-AEAA-7F265BDC07CE}"/>
     <hyperlink ref="F9" r:id="rId8" location="contrast-minimum" xr:uid="{B7094FDD-1C54-49B5-81A5-957754EFEB60}"/>
     <hyperlink ref="F10" r:id="rId9" location="consistent-navigation" xr:uid="{61432BEA-AFD2-4E9B-A153-619782D49F58}"/>
+    <hyperlink ref="F13" r:id="rId10" xr:uid="{9D134B1A-4F6D-447C-97CA-2165353E4E66}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
Issue SEO-4 and SEO-5 in SEO Template implemented.
</commit_message>
<xml_diff>
--- a/Template-SEO-audit.xlsx
+++ b/Template-SEO-audit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicopatsch/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="434" documentId="11_05D6EA6CE7DA307BAFC13D42CE951501BDC39C52" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{691B2F65-EBC8-47DC-AB28-15FFCC8C5525}"/>
+  <xr:revisionPtr revIDLastSave="513" documentId="11_05D6EA6CE7DA307BAFC13D42CE951501BDC39C52" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6422BC6-F4EB-4B18-8EDE-3C85370847CD}"/>
   <bookViews>
     <workbookView xWindow="940" yWindow="460" windowWidth="27860" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="105">
   <si>
     <t>Category</t>
   </si>
@@ -415,7 +415,7 @@
     <t>SEO-4</t>
   </si>
   <si>
-    <t>Line 44: Putting keywords in a hidden div. This considered "black hat" technique</t>
+    <t>Line 44: Putting keywords in a hidden div. This considered "black hat" technique.</t>
   </si>
   <si>
     <t>I strongly advise against using black hat SEO techniques on an established company’s website. You run the risk of having your website excluded from Google search results.</t>
@@ -428,6 +428,78 @@
   </si>
   <si>
     <t>SEO-5</t>
+  </si>
+  <si>
+    <t>Line 95:Putting keywords in alt attributes without it making sense for the reader called "keyword stuffing". This also considered "black hat" technique.</t>
+  </si>
+  <si>
+    <t>Use keywords that related to the image but also describes it for the reader.
+ For example in green -&gt;</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">   alt="Drawing of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Atlanta web designer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> Mike"</t>
+    </r>
+  </si>
+  <si>
+    <t>SEO-6</t>
+  </si>
+  <si>
+    <t>Useing the  background-image property in CSS rather than IMG tag in HTML</t>
+  </si>
+  <si>
+    <t>This is a performance issue. But googleing it, there were mixed opinions on the matter.</t>
+  </si>
+  <si>
+    <t>SEO-7</t>
+  </si>
+  <si>
+    <t>Line 95: Image size is too big for it's container.</t>
+  </si>
+  <si>
+    <t>The larger the image, the bigger the file, and the longer it takes for a browser to download.</t>
+  </si>
+  <si>
+    <t>It's important to resize images before uploading them to your website. Use approrpiate sizes, one that's close to it's containers size. You can also use tools that compress an image, to further reduce the image in size. Free tools for example: https://www.befunky.com/create/resize-image/ and https://compressor.io/</t>
+  </si>
+  <si>
+    <t>Use to tools to resize "atlanta web designer mike.png" to the size of its container(no smaller than 100x102 px, keeping aspect ratio). Than compress it with https://compressor.io/ tool and finally replace the new resized_compressed version with the original.</t>
+  </si>
+  <si>
+    <t>SEO-8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Css and Javascript files are not minifed. </t>
+  </si>
+  <si>
+    <t>Minifying a file means removing unnecessary characters (spaces, line breaks, comments, block separators) from the file, which drastically reduces its file size. The smaller the file sizes, the faster a browser can load them and less time it takes crawlers to index your pages.</t>
+  </si>
+  <si>
+    <t>Use a tool like https://www.minifier.org/ to minify your css and javascript files when you can.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Follow the link https://www.minifier.org/ . Copy paste your css code in the text field, press minify, and copy paste the new code into your css file(or make a new css file for minifed version), put the new file in your directory and modify the path in your html to excess the new css file. </t>
   </si>
   <si>
     <t>Supplimentary info:</t>
@@ -579,7 +651,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -798,8 +872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -1118,7 +1192,7 @@
       </c>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:26" s="13" customFormat="1" ht="146.25">
+    <row r="15" spans="1:26" ht="146.25">
       <c r="A15" s="12" t="s">
         <v>81</v>
       </c>
@@ -1136,34 +1210,82 @@
       </c>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:26" ht="15.75">
+    <row r="16" spans="1:26" ht="129">
       <c r="A16" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
+      <c r="B16" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>89</v>
+      </c>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6" ht="15.75">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
+    <row r="17" spans="1:6" ht="64.5">
+      <c r="A17" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="11"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="18" spans="1:6" ht="194.25">
+      <c r="A18" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="1:6" ht="178.5">
+      <c r="A19" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="F19" s="6"/>
+    </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1"/>
     <row r="21" spans="1:6" ht="15.75" customHeight="1"/>
     <row r="22" spans="1:6" ht="113.25">
       <c r="A22" s="6" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>

</xml_diff>

<commit_message>
Issue SEO-6 and SEO-7 in SEO Template implemented.
</commit_message>
<xml_diff>
--- a/Template-SEO-audit.xlsx
+++ b/Template-SEO-audit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicopatsch/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="513" documentId="11_05D6EA6CE7DA307BAFC13D42CE951501BDC39C52" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6422BC6-F4EB-4B18-8EDE-3C85370847CD}"/>
+  <xr:revisionPtr revIDLastSave="570" documentId="11_05D6EA6CE7DA307BAFC13D42CE951501BDC39C52" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4EF0B6AA-32C6-4743-A255-1B9F473C0B38}"/>
   <bookViews>
     <workbookView xWindow="940" yWindow="460" windowWidth="27860" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="112">
   <si>
     <t>Category</t>
   </si>
@@ -466,46 +466,91 @@
     <t>SEO-6</t>
   </si>
   <si>
+    <t>Line 95: Image size is too big for it's container.</t>
+  </si>
+  <si>
+    <t>The larger the image, the bigger the file, and the longer it takes for a browser to download.</t>
+  </si>
+  <si>
+    <t>It's important to resize images before uploading them to your website. Use approrpiate sizes, one that's close to it's containers size. You can also use tools that compress an image, to further reduce the image in size. Free tools for example: https://www.befunky.com/create/resize-image/ and https://compressor.io/</t>
+  </si>
+  <si>
+    <t>Use to tools to resize "atlanta web designer mike.png" to the size of its container(no smaller than 100x102 px, keeping aspect ratio). Than compress it with https://compressor.io/ tool and finally replace the new resized_compressed version with the original.</t>
+  </si>
+  <si>
+    <t>SEO-7</t>
+  </si>
+  <si>
+    <t>Line 24: Resources are blocking the first paint of the page.</t>
+  </si>
+  <si>
+    <t>If you reduce the number of render blocking resources, you can shorten the critical rendering path and reduce page load times, thus improving the user experience and search engine optimization. Use the Coverage tab in Chrome DevTools to identify non-critical CSS and JS.</t>
+  </si>
+  <si>
+    <t>For JS: We can use the defer and async attributes of the &lt;script&gt; tag. They make scripts added to the &lt;head&gt; section of an HTML document non-render blocking, but in a different way; deferred scripts respect the document order while asynchronous scripts are independent of the DOM.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Change the code to:
+  &lt;script </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>async</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> src="./js/jquery-2.1.0.js"&gt;&lt;/script&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>https://blog.logrocket.com/9-tricks-eliminate-render-blocking-resources/</t>
+  </si>
+  <si>
+    <t>SEO-8</t>
+  </si>
+  <si>
+    <t>Line 19: Resources are blocking the first paint of the page.</t>
+  </si>
+  <si>
+    <t>SEO-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Css and Javascript files are not minifed. </t>
+  </si>
+  <si>
+    <t>Minifying a file means removing unnecessary characters (spaces, line breaks, comments, block separators) from the file, which drastically reduces its file size. The smaller the file sizes, the faster a browser can load them and less time it takes crawlers to index your pages.</t>
+  </si>
+  <si>
+    <t>Use a tool like https://www.minifier.org/ to minify your css and javascript files when you can.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Follow the link https://www.minifier.org/ . Copy paste your css code in the text field, press minify, and copy paste the new code into your css file(or make a new css file for minifed version), put the new file in your directory and modify the path in your html to excess the new css file. </t>
+  </si>
+  <si>
+    <t>Supplimentary info:</t>
+  </si>
+  <si>
+    <t>Line number references are from the code "Indentation style changes in code (personal pref)" commit not from the original version of the code, for easier comparison with the amended version.</t>
+  </si>
+  <si>
     <t>Useing the  background-image property in CSS rather than IMG tag in HTML</t>
   </si>
   <si>
     <t>This is a performance issue. But googleing it, there were mixed opinions on the matter.</t>
-  </si>
-  <si>
-    <t>SEO-7</t>
-  </si>
-  <si>
-    <t>Line 95: Image size is too big for it's container.</t>
-  </si>
-  <si>
-    <t>The larger the image, the bigger the file, and the longer it takes for a browser to download.</t>
-  </si>
-  <si>
-    <t>It's important to resize images before uploading them to your website. Use approrpiate sizes, one that's close to it's containers size. You can also use tools that compress an image, to further reduce the image in size. Free tools for example: https://www.befunky.com/create/resize-image/ and https://compressor.io/</t>
-  </si>
-  <si>
-    <t>Use to tools to resize "atlanta web designer mike.png" to the size of its container(no smaller than 100x102 px, keeping aspect ratio). Than compress it with https://compressor.io/ tool and finally replace the new resized_compressed version with the original.</t>
-  </si>
-  <si>
-    <t>SEO-8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Css and Javascript files are not minifed. </t>
-  </si>
-  <si>
-    <t>Minifying a file means removing unnecessary characters (spaces, line breaks, comments, block separators) from the file, which drastically reduces its file size. The smaller the file sizes, the faster a browser can load them and less time it takes crawlers to index your pages.</t>
-  </si>
-  <si>
-    <t>Use a tool like https://www.minifier.org/ to minify your css and javascript files when you can.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Follow the link https://www.minifier.org/ . Copy paste your css code in the text field, press minify, and copy paste the new code into your css file(or make a new css file for minifed version), put the new file in your directory and modify the path in your html to excess the new css file. </t>
-  </si>
-  <si>
-    <t>Supplimentary info:</t>
-  </si>
-  <si>
-    <t>Line number references are from the code "Indentation style changes in code (personal pref)" commit not from the original version of the code, for easier comparison with the amended version.</t>
   </si>
 </sst>
 </file>
@@ -873,7 +918,7 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -1228,64 +1273,84 @@
       </c>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6" ht="64.5">
+    <row r="17" spans="1:6" ht="194.25">
       <c r="A17" s="12" t="s">
         <v>90</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="D17" s="11"/>
-      <c r="E17" s="6"/>
+      <c r="D17" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>94</v>
+      </c>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6" ht="194.25">
+    <row r="18" spans="1:6" ht="205.5" customHeight="1">
       <c r="A18" s="12" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>96</v>
+        <v>97</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>98</v>
       </c>
       <c r="E18" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="205.5" customHeight="1">
+      <c r="A19" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="F18" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="5" t="s">
+        <v>100</v>
+      </c>
     </row>
-    <row r="19" spans="1:6" ht="178.5">
-      <c r="A19" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="F19" s="6"/>
+    <row r="21" spans="1:6" ht="178.5">
+      <c r="A21" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="F21" s="6"/>
     </row>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1"/>
     <row r="22" spans="1:6" ht="113.25">
       <c r="A22" s="6" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
@@ -1293,7 +1358,20 @@
       <c r="F22" s="6"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="24" spans="1:6" ht="64.5">
+      <c r="A24" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D24" s="11"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+    </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1"/>
     <row r="26" spans="1:6" ht="15.75" customHeight="1"/>
     <row r="27" spans="1:6" ht="15.75" customHeight="1"/>
@@ -2283,6 +2361,8 @@
     <hyperlink ref="F9" r:id="rId8" location="contrast-minimum" xr:uid="{B7094FDD-1C54-49B5-81A5-957754EFEB60}"/>
     <hyperlink ref="F10" r:id="rId9" location="consistent-navigation" xr:uid="{61432BEA-AFD2-4E9B-A153-619782D49F58}"/>
     <hyperlink ref="F13" r:id="rId10" xr:uid="{9D134B1A-4F6D-447C-97CA-2165353E4E66}"/>
+    <hyperlink ref="F18" r:id="rId11" xr:uid="{43FEEA1C-9F19-44BE-AC03-C36B4EC3F43C}"/>
+    <hyperlink ref="F19" r:id="rId12" xr:uid="{6CEDF922-0E98-44C7-8CB3-CA5D7F6F7CF1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
Issue SEO-8 and SEO-9 in SEO Template implemented.
</commit_message>
<xml_diff>
--- a/Template-SEO-audit.xlsx
+++ b/Template-SEO-audit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicopatsch/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="570" documentId="11_05D6EA6CE7DA307BAFC13D42CE951501BDC39C52" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4EF0B6AA-32C6-4743-A255-1B9F473C0B38}"/>
+  <xr:revisionPtr revIDLastSave="605" documentId="11_05D6EA6CE7DA307BAFC13D42CE951501BDC39C52" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34A6E172-AA39-49E0-BF2C-8765EDD38D63}"/>
   <bookViews>
     <workbookView xWindow="940" yWindow="460" windowWidth="27860" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="122">
   <si>
     <t>Category</t>
   </si>
@@ -463,7 +463,8 @@
     </r>
   </si>
   <si>
-    <t>SEO-6</t>
+    <t>SEO-6/
+Performance</t>
   </si>
   <si>
     <t>Line 95: Image size is too big for it's container.</t>
@@ -478,7 +479,8 @@
     <t>Use to tools to resize "atlanta web designer mike.png" to the size of its container(no smaller than 100x102 px, keeping aspect ratio). Than compress it with https://compressor.io/ tool and finally replace the new resized_compressed version with the original.</t>
   </si>
   <si>
-    <t>SEO-7</t>
+    <t>SEO-7/
+Performance</t>
   </si>
   <si>
     <t>Line 24: Resources are blocking the first paint of the page.</t>
@@ -505,7 +507,7 @@
         <color rgb="FF00B050"/>
         <rFont val="Calibri"/>
       </rPr>
-      <t>async</t>
+      <t>defer</t>
     </r>
     <r>
       <rPr>
@@ -520,13 +522,58 @@
     <t>https://blog.logrocket.com/9-tricks-eliminate-render-blocking-resources/</t>
   </si>
   <si>
-    <t>SEO-8</t>
+    <t>SEO-8/
+Performance</t>
   </si>
   <si>
     <t>Line 19: Resources are blocking the first paint of the page.</t>
   </si>
   <si>
-    <t>SEO-10</t>
+    <t xml:space="preserve">For CSS: We can split CSS into critical and non-critical parts. This is a performance optimization technique and you can do this manually but I recommend to use tools like: https://www.sitelocity.com/critical-path-css-generator to make this job easy. </t>
+  </si>
+  <si>
+    <t>Follow the link https://www.sitelocity.com/critical-path-css-generator and follow the instructions provided.</t>
+  </si>
+  <si>
+    <t>SEO-9</t>
+  </si>
+  <si>
+    <t>Tap targets are not sized appropriately</t>
+  </si>
+  <si>
+    <t>Tap targets are the areas of a web page that users on touch devices can interact with. Buttons, links, and form elements all have tap targets.
+Many search engines rank pages based on how mobile-friendly they are. Making sure tap targets are big enough and far enough apart from each other makes your page more mobile-friendly and accessible.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Make sure there is enough space between elements that are tap targets. Targets that are smaller than 48 px by 48 px or closer than 8 px apart fail the audit. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>(Rephrase this?)</t>
+    </r>
+  </si>
+  <si>
+    <t>Add the code in your CSS:
+footer li {
+  margin: 10px 0;
+}</t>
+  </si>
+  <si>
+    <t>https://web.dev/tap-targets/?utm_source=lighthouse&amp;utm_medium=devtools</t>
+  </si>
+  <si>
+    <t>SEO-10/
+Performance</t>
   </si>
   <si>
     <t xml:space="preserve">Css and Javascript files are not minifed. </t>
@@ -547,10 +594,16 @@
     <t>Line number references are from the code "Indentation style changes in code (personal pref)" commit not from the original version of the code, for easier comparison with the amended version.</t>
   </si>
   <si>
+    <t>SEO-6</t>
+  </si>
+  <si>
     <t>Useing the  background-image property in CSS rather than IMG tag in HTML</t>
   </si>
   <si>
     <t>This is a performance issue. But googleing it, there were mixed opinions on the matter.</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -917,8 +970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -1274,7 +1327,7 @@
       <c r="F16" s="6"/>
     </row>
     <row r="17" spans="1:6" ht="194.25">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="6" t="s">
         <v>90</v>
       </c>
       <c r="B17" s="6" t="s">
@@ -1292,7 +1345,7 @@
       <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:6" ht="205.5" customHeight="1">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="6" t="s">
         <v>95</v>
       </c>
       <c r="B18" s="6" t="s">
@@ -1312,7 +1365,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="205.5" customHeight="1">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="6" t="s">
         <v>101</v>
       </c>
       <c r="B19" s="6" t="s">
@@ -1321,36 +1374,60 @@
       <c r="C19" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
+      <c r="D19" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>104</v>
+      </c>
       <c r="F19" s="5" t="s">
         <v>100</v>
       </c>
     </row>
+    <row r="20" spans="1:6" ht="243">
+      <c r="A20" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
     <row r="21" spans="1:6" ht="178.5">
-      <c r="A21" s="12" t="s">
-        <v>103</v>
+      <c r="A21" s="6" t="s">
+        <v>111</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="F21" s="6"/>
     </row>
     <row r="22" spans="1:6" ht="113.25">
       <c r="A22" s="6" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
@@ -1360,15 +1437,17 @@
     <row r="23" spans="1:6" ht="15.75" customHeight="1"/>
     <row r="24" spans="1:6" ht="64.5">
       <c r="A24" s="12" t="s">
-        <v>90</v>
+        <v>118</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="D24" s="11"/>
+        <v>120</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>121</v>
+      </c>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
     </row>
@@ -2363,6 +2442,7 @@
     <hyperlink ref="F13" r:id="rId10" xr:uid="{9D134B1A-4F6D-447C-97CA-2165353E4E66}"/>
     <hyperlink ref="F18" r:id="rId11" xr:uid="{43FEEA1C-9F19-44BE-AC03-C36B4EC3F43C}"/>
     <hyperlink ref="F19" r:id="rId12" xr:uid="{6CEDF922-0E98-44C7-8CB3-CA5D7F6F7CF1}"/>
+    <hyperlink ref="F20" r:id="rId13" xr:uid="{D90F8BF8-4C36-40F5-96C1-2BCFAF65F3D4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
Added ScrollToTop button on home page and aria landmarks for both
</commit_message>
<xml_diff>
--- a/Template-SEO-audit.xlsx
+++ b/Template-SEO-audit.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25825"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25910"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicopatsch/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="605" documentId="11_05D6EA6CE7DA307BAFC13D42CE951501BDC39C52" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34A6E172-AA39-49E0-BF2C-8765EDD38D63}"/>
+  <xr:revisionPtr revIDLastSave="944" documentId="11_05D6EA6CE7DA307BAFC13D42CE951501BDC39C52" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72D166D4-3F39-4315-AF35-AE16BFDE4520}"/>
   <bookViews>
     <workbookView xWindow="940" yWindow="460" windowWidth="27860" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="140">
   <si>
     <t>Category</t>
   </si>
@@ -92,8 +92,23 @@
     <t>Add titles to web pages that describe topic or purpose.</t>
   </si>
   <si>
-    <t>Change code to something like:
-    &lt;title&gt;Freelance Web Design Services by Mike in Atlanta&lt;/title&gt;</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Change code to something like:
+  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">    &lt;title&gt;Websites and graphic design - GoMike Designs&lt;/title&gt;</t>
+    </r>
   </si>
   <si>
     <t>https://webaim.org/standards/wcag/checklist#sc2.4.2</t>
@@ -111,7 +126,23 @@
     <t>Ensure that the alternative text for the image or image input provides a succinct, yet equivalent alternative to the content and function of the image. Screen readers and browser presentation inform the user that the object is an image, so alternative text of "image of..." (and similar) should be avoided. If the image does not convey content or if the content is presented in nearby text (e.g., a caption), null/empty alternative text (alt="") is appropriate.</t>
   </si>
   <si>
-    <t>If caption tag functions: (alt="")</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Change code to something like:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>alt="Woman walking a fluffy white dog. On click enlarge picture"</t>
+    </r>
   </si>
   <si>
     <t>https://webaim.org/standards/wcag/checklist#sc1.1.1</t>
@@ -178,8 +209,8 @@
     <t>https://www.w3.org/WAI/WCAG21/quickref/?showtechniques=311%2C131#info-and-relationships</t>
   </si>
   <si>
-    <t>&lt;- Situation A: H71
-&lt;- Replicate the OC example with fieldset</t>
+    <t xml:space="preserve">&lt;- Situation A: H71
+</t>
   </si>
   <si>
     <t>Accessibility-6</t>
@@ -244,13 +275,14 @@
     <t>Accessibility-7</t>
   </si>
   <si>
-    <t>Line 122,171: If the same visual presentation can be made using text alone, an image is not used to present that text.</t>
+    <t>Line 122,171: If the same visual presentation can be achieved using text alone, an image is not to be used to present that text.</t>
   </si>
   <si>
     <t xml:space="preserve"> It prevents people from modifying fonts and doesn’t respond to changes in color, size, and regular text. It also means readers can’t select the text if they need to copy or annotate it. Finally, while it is possible to communicate all of the text in the image as alternative text, this often isn’t done in practice(the alt text was  insufficient here as well), so assistive technology users can’t perceive the content.</t>
   </si>
   <si>
-    <t>C22: Using CSS to control visual presentation of text.
+    <t>Always hardcode text in HTML and stlye it with CSS if possible. Detaild practices in reference: C22: Using CSS to control visual presentation of text. 
+Alternative solution(not recommended): Provide alt text that contains exactly the same text as on the picture.
 C30: Using CSS to replace text with images of text and providing user interface controls to switch</t>
   </si>
   <si>
@@ -290,28 +322,99 @@
     <t>If your navigation contains certain functionality on some pages but not on others (i.e., a profile menu or a logo that takes users to the homepage), it could be disorienting even if the items are presented in the same relative order.</t>
   </si>
   <si>
-    <t>G61: Presenting repeated components in the same relative order each time they appear</t>
-  </si>
-  <si>
-    <t>Fix the nav bar on page2 to look and work the same as in the homepage.</t>
+    <t>Make sure your navigation elements are consistent meaning: they have the same text, appearance and follow the same order on all the pages.
+  Detaild practices in reference: G61: Presenting repeated components in the same relative order each time they appear</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>The path for the resources were erroneous, the file the browser were looking for was non existing, so the browser couldn't load the css and javascript files.  
+Change all the files with .min like:  &lt;script src="./js/jquery-2.1.0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>.min</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">.js"&gt;&lt;/script&gt; to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">&lt;script src="./js/jquery-2.1.0.js"&gt;&lt;/script&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>or add the proper resources( in this case the minified files) to the appropriate folders.</t>
+    </r>
   </si>
   <si>
     <t>https://www.w3.org/WAI/WCAG21/quickref/?showtechniques=323#consistent-navigation</t>
   </si>
   <si>
-    <t>Maybe this is not an accessability issue. As I could found it with TAB key. But it's an issue</t>
-  </si>
-  <si>
     <t>Accessibility-10</t>
   </si>
   <si>
-    <t>F63: Failure of Success Criterion 2.4.4 due to providing link context only in content that is not related to the link</t>
+    <t>Line59: Link text is insufficient</t>
+  </si>
+  <si>
+    <t>The text of the link doesn't describe the purpuse of the link. This can introduce confusion not just for keyboard and screen reader users but for anybody.</t>
+  </si>
+  <si>
+    <t>Make sure the text of a link  describes the destination in a short and simple way. If it's not possible to have text for a link for let say styling reasons, use aria-label attribute to describe the purpose of the link.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Change the code to something like:
+      href="page2.html"&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Contact page</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>&lt;/a</t>
+    </r>
   </si>
   <si>
     <t>SEO-1</t>
   </si>
   <si>
-    <t>Line 122, issue-1: Image element was used instead of H1 element for the "main title"/theme of the page.</t>
+    <t>Line 121, issue-1: Image element was used instead of H1 element for the "main title"/theme of the page.</t>
   </si>
   <si>
     <t>The h1 element helps defining the main content/keywords regards what the page is all about to search engines.(Similarly to the title tag, but there is some differences)</t>
@@ -326,7 +429,9 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
       </rPr>
-      <t xml:space="preserve">&lt;title&gt; </t>
+      <t xml:space="preserve">
+Change the img tag to an h1 and hardcode the text:
+&lt;h1&gt; I create </t>
     </r>
     <r>
       <rPr>
@@ -334,6 +439,23 @@
         <color rgb="FF00B050"/>
         <rFont val="Calibri"/>
       </rPr>
+      <t>websites and graphic design</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> that help Atlanta companies become attractive and recognizable online. &lt;/h1&gt;
+(keywords in green) &lt;title&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+      </rPr>
       <t>Websites and graphic design</t>
     </r>
     <r>
@@ -342,8 +464,33 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
       </rPr>
-      <t xml:space="preserve"> - GoMike Designs &lt;/title&gt;
-&lt;h1&gt; I create </t>
+      <t xml:space="preserve"> - GoMike Designs &lt;/title&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>https://moz.com/blog/h1-seo-experiment</t>
+  </si>
+  <si>
+    <t>SEO-2</t>
+  </si>
+  <si>
+    <t>Line 121, issue-2:Responsiveness was not set for this element.</t>
+  </si>
+  <si>
+    <t>Google now uses the mobile version of your site (if it exists) as the primary version for indexing purposes. The better the mobile version of your site performs, the more likely will appear higher in search results. So if you don't have a mobile verision responsivness is a must for SEO.</t>
+  </si>
+  <si>
+    <t>In this case I changed the IMG element to an h1 which makes it automatically responsive, but the font size can be quite cramped if it's large enough on smaller screens like mobile, so I set the font size in CSS to change depending on the viewwidth of the page.
+For your images here is a guide how to make them responsive: https://www.freecodecamp.org/news/css-responsive-image-tutorial/</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">I added the following code to the css file: </t>
     </r>
     <r>
       <rPr>
@@ -351,7 +498,9 @@
         <color rgb="FF00B050"/>
         <rFont val="Calibri"/>
       </rPr>
-      <t>websites and graphic design</t>
+      <t xml:space="preserve">h1 {
+font-size: clamp(1.8em, 3.2vw, 2.5em);}
+</t>
     </r>
     <r>
       <rPr>
@@ -359,48 +508,17 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
       </rPr>
-      <t xml:space="preserve"> that help Atlanta companies become attractive and recognizable online. &lt;/h1&gt;</t>
-    </r>
-  </si>
-  <si>
-    <t>SEO-2</t>
-  </si>
-  <si>
-    <t>Line 122, issue-2:Responsiveness was not set for this element.</t>
-  </si>
-  <si>
-    <t>Google now uses the mobile version of your site (if it exists) as the primary version for indexing purposes. The better the mobile version of your site performs, the more likely will appear higher in search results. So if you don't have a mobile verision responsivness is a must for SEO.</t>
-  </si>
-  <si>
-    <t>If you have the budget make a mobile version of your site.If not, it's ok just code your webpages mobile-first, than adapt to tablet and desktop. Google will appreciate this and get you higher in his search results.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve">Change the img tag to an h1 and hardcode the text:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>&lt;h1&gt; I create websites and design graphics that help Atlanta companies become attractive and recognizable online. &lt;/h1&gt;</t>
+      <t>clamp() is great for responsive text because it has a minimum, middle and a maximum value. It's also best to use relative sizes over absolute ones.</t>
     </r>
   </si>
   <si>
     <t>https://developers.google.com/search/mobile-sites/mobile-first-indexing</t>
   </si>
   <si>
-    <t>SEO-3</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Missing good sematic stracture.(mostly just dives, instead of header,main, footer etc.)</t>
+    <t>SEO-3/Accessibility</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Missing good sematic markup.(mostly just dives, instead of header,main, footer etc.)</t>
   </si>
   <si>
     <t xml:space="preserve"> Semantic tags makes web pages more informative and adaptable, allowing browsers and search engines to better interpret content. </t>
@@ -412,19 +530,25 @@
     <t>For example: Add Header, main, section and footer semantic tags (Check amended code).</t>
   </si>
   <si>
+    <t>https://developer.mozilla.org/en-US/docs/Learn/Accessibility/HTML</t>
+  </si>
+  <si>
     <t>SEO-4</t>
   </si>
   <si>
     <t>Line 44: Putting keywords in a hidden div. This considered "black hat" technique.</t>
   </si>
   <si>
-    <t>I strongly advise against using black hat SEO techniques on an established company’s website. You run the risk of having your website excluded from Google search results.</t>
+    <t>I strongly advise against using black hat SEO techniques on your website. You run the risk of having your website excluded from Google search results.</t>
   </si>
   <si>
     <t>Place your keywords in your title tag, description, h1,h2...etc. elements, paragraphs and image alt attribute, in a way it's also natural for the reader. (Otherwise its "keyword stuffing" and is considered a black hat technique as well.)</t>
   </si>
   <si>
     <t>Remove divs with keywords classes.</t>
+  </si>
+  <si>
+    <t>https://www.searchenginejournal.com/11-black-hat-techniques-can-kill-seo-campaign/180601/#close</t>
   </si>
   <si>
     <t>SEO-5</t>
@@ -476,7 +600,10 @@
     <t>It's important to resize images before uploading them to your website. Use approrpiate sizes, one that's close to it's containers size. You can also use tools that compress an image, to further reduce the image in size. Free tools for example: https://www.befunky.com/create/resize-image/ and https://compressor.io/</t>
   </si>
   <si>
-    <t>Use to tools to resize "atlanta web designer mike.png" to the size of its container(no smaller than 100x102 px, keeping aspect ratio). Than compress it with https://compressor.io/ tool and finally replace the new resized_compressed version with the original.</t>
+    <t>Use to tools to resize "atlanta web designer mike.png" to the size of its container(no smaller than 100x102 px, keeping aspect ratio). Than compress it with https://compressor.io/ tool and finally replace the new resized_compressed version with the original and define the new path in the HTML code.</t>
+  </si>
+  <si>
+    <t>https://web.dev/compress-images/</t>
   </si>
   <si>
     <t>SEO-7/
@@ -486,10 +613,10 @@
     <t>Line 24: Resources are blocking the first paint of the page.</t>
   </si>
   <si>
-    <t>If you reduce the number of render blocking resources, you can shorten the critical rendering path and reduce page load times, thus improving the user experience and search engine optimization. Use the Coverage tab in Chrome DevTools to identify non-critical CSS and JS.</t>
-  </si>
-  <si>
-    <t>For JS: We can use the defer and async attributes of the &lt;script&gt; tag. They make scripts added to the &lt;head&gt; section of an HTML document non-render blocking, but in a different way; deferred scripts respect the document order while asynchronous scripts are independent of the DOM.</t>
+    <t>If you reduce the number of render blocking resources, you can shorten the critical rendering path and reduce page load times, thus improving the user experience and search engine optimization.</t>
+  </si>
+  <si>
+    <t>For JS: First use the Coverage tab in Chrome DevTools to identify non-critical CSS and JS.We can use the defer and async attributes of the &lt;script&gt; tag. They make scripts added to the &lt;head&gt; section of an HTML document non-render blocking, but in a different way; deferred scripts respect the document order while asynchronous scripts are independent of the DOM.</t>
   </si>
   <si>
     <r>
@@ -522,17 +649,50 @@
     <t>https://blog.logrocket.com/9-tricks-eliminate-render-blocking-resources/</t>
   </si>
   <si>
-    <t>SEO-8/
-Performance</t>
-  </si>
-  <si>
-    <t>Line 19: Resources are blocking the first paint of the page.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">For CSS: We can split CSS into critical and non-critical parts. This is a performance optimization technique and you can do this manually but I recommend to use tools like: https://www.sitelocity.com/critical-path-css-generator to make this job easy. </t>
-  </si>
-  <si>
-    <t>Follow the link https://www.sitelocity.com/critical-path-css-generator and follow the instructions provided.</t>
+    <t>SEO-8</t>
+  </si>
+  <si>
+    <t>Page2, line 6:Document does not have a meta description</t>
+  </si>
+  <si>
+    <t>The &lt;meta name="description"&gt; element provides a summary of a page's content that search engines include in search results. A high-quality, unique meta description makes your page appear more relevant and can increase your search traffic.</t>
+  </si>
+  <si>
+    <t>- Use a unique description for each page.
+ - Make descriptions clear and concise. Avoid vague descriptions like "Home."
+- Avoid keyword stuffing. It doesn't help users, and search engines may mark the page as spam.
+- Descriptions don't have to be complete sentences; they can contain structured data.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>&lt;meta
+      name="description"
+      content="</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Looking to impove your website with a new graphic design? Perhaps a new logo for your company? I would love to help, contact me today!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>" /&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>https://web.dev/meta-description/?utm_source=lighthouse&amp;utm_medium=devtools</t>
   </si>
   <si>
     <t>SEO-9</t>
@@ -545,28 +705,30 @@
 Many search engines rank pages based on how mobile-friendly they are. Making sure tap targets are big enough and far enough apart from each other makes your page more mobile-friendly and accessible.</t>
   </si>
   <si>
+    <t>Make sure there is enough space between elements that are tap targets. Targets has to be at least 48 px by 48 px or further apart than 8 px from each other.</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
       </rPr>
-      <t xml:space="preserve">Make sure there is enough space between elements that are tap targets. Targets that are smaller than 48 px by 48 px or closer than 8 px apart fail the audit. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>(Rephrase this?)</t>
-    </r>
-  </si>
-  <si>
-    <t>Add the code in your CSS:
-footer li {
-  margin: 10px 0;
+      <t xml:space="preserve">Add the code in your CSS:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>@media (max-width: 1279px) {
+  footer li {
+    margin: 10px 0;
+  }
 }</t>
+    </r>
   </si>
   <si>
     <t>https://web.dev/tap-targets/?utm_source=lighthouse&amp;utm_medium=devtools</t>
@@ -582,10 +744,58 @@
     <t>Minifying a file means removing unnecessary characters (spaces, line breaks, comments, block separators) from the file, which drastically reduces its file size. The smaller the file sizes, the faster a browser can load them and less time it takes crawlers to index your pages.</t>
   </si>
   <si>
-    <t>Use a tool like https://www.minifier.org/ to minify your css and javascript files when you can.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Follow the link https://www.minifier.org/ . Copy paste your css code in the text field, press minify, and copy paste the new code into your css file(or make a new css file for minifed version), put the new file in your directory and modify the path in your html to excess the new css file. </t>
+    <t>Use a tool like CSSNano to minify css -https://github.com/cssnano/cssnano and UglifyJS to minify JavaScript  - https://github.com/mishoo/UglifyJS via Command line
+ or
+https://www.minifier.org/ to minify your css and javascript files online.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There is installation guide for both CSSNano annd UglifyJS in the link provided.
+For https://www.minifier.org/ . Copy paste your css code in the text field, press minify, and copy paste the new code into your css file(or make a new css file for minifed version), put the new file in your directory and modify the path in your html to excess the new css file. </t>
+  </si>
+  <si>
+    <t>https://web.dev/reduce-network-payloads-using-text-compression/</t>
+  </si>
+  <si>
+    <t>SEO-11</t>
+  </si>
+  <si>
+    <t>Useing lot's of directory links doesn't help SEO. The ones you have doesn't seem professional etiher or relevent to your content.</t>
+  </si>
+  <si>
+    <t>If there are free quality directory listings for your area of expertise, feel free to submit your info. Even though nowadays this won’t help much with you SEO, it is quick and easy to do.
+It will show Google that people are talking about you.</t>
+  </si>
+  <si>
+    <t>Instead of so many links pointing to directories, better outbound links would be ones using businesses you worked with. 
+Use only links that are quality.  Weave them in the articles/paragraphs of the page in a natural way rather than place them in the footer. In this way they be more likely to get more attention and clicks.</t>
+  </si>
+  <si>
+    <t>For example, you could make links from the titles of the websites you designed. Ergo, turn this into a link: "Website for a Atlanta's Premier dog sitters"</t>
+  </si>
+  <si>
+    <t>https://www.searchenginejournal.com/link-building-guide/online-directories/</t>
+  </si>
+  <si>
+    <t>SEO-12</t>
+  </si>
+  <si>
+    <t>The website seem to lack good, "quailty" links.</t>
+  </si>
+  <si>
+    <t>Quality over quantity, just having as many links as possible doesn't improve your SEO. In fact if they are just made without realting much to you content they considered black hat. It's also important where you place them.</t>
+  </si>
+  <si>
+    <t>A quality link:
+- Originates on a popular or high-quality website.
+- Is found among content that is relevant to your profession.
+- Attracts real traffic, meaning that it is on a page real visitors read, not hidden away in some obscure part of the website.
+Best to worste where you should have your links for better ranking: Homepage, secondary page, blog post and than footers,sidebars, pages listing partner websites.</t>
+  </si>
+  <si>
+    <t>The best links are inbound links for SEO. You could obtain these by asking nicely businesses you already worked with to include your websites link on there page somewhere, or in their blog or social media site if they have any.</t>
+  </si>
+  <si>
+    <t>https://www.searchenginejournal.com/seo-guide/why-links-important-seo/</t>
   </si>
   <si>
     <t>Supplimentary info:</t>
@@ -594,23 +804,14 @@
     <t>Line number references are from the code "Indentation style changes in code (personal pref)" commit not from the original version of the code, for easier comparison with the amended version.</t>
   </si>
   <si>
-    <t>SEO-6</t>
-  </si>
-  <si>
-    <t>Useing the  background-image property in CSS rather than IMG tag in HTML</t>
-  </si>
-  <si>
-    <t>This is a performance issue. But googleing it, there were mixed opinions on the matter.</t>
-  </si>
-  <si>
-    <t>?</t>
+    <t>Simply put, the more quality links you have, the higher your authority, and therefore, the better your ranking is.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -678,6 +879,13 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF444444"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -713,7 +921,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -752,6 +960,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -970,8 +1179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -1199,7 +1408,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="146.25">
+    <row r="10" spans="1:26" ht="209.25" customHeight="1">
       <c r="A10" s="6" t="s">
         <v>56</v>
       </c>
@@ -1212,247 +1421,305 @@
       <c r="D10" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="13" t="s">
         <v>60</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="10"/>
+    </row>
+    <row r="11" spans="1:26" ht="180" customHeight="1">
+      <c r="A11" s="6" t="s">
         <v>62</v>
       </c>
+      <c r="B11" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="11" spans="1:26" ht="64.5">
-      <c r="A11" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="5"/>
+    <row r="12" spans="1:26" ht="162">
+      <c r="A12" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G12" s="6"/>
     </row>
-    <row r="12" spans="1:26" ht="201.75" customHeight="1">
-      <c r="A12" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="1:26" ht="194.25">
+    <row r="13" spans="1:26" ht="275.25">
       <c r="A13" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>71</v>
+        <v>73</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="96.75">
       <c r="A14" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>77</v>
+        <v>79</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>80</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="F14" s="5"/>
+        <v>83</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G14" s="11"/>
     </row>
     <row r="15" spans="1:26" ht="146.25">
       <c r="A15" s="12" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="F15" s="6"/>
+        <v>89</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>90</v>
+      </c>
     </row>
-    <row r="16" spans="1:26" ht="129">
+    <row r="16" spans="1:26" ht="113.25">
       <c r="A16" s="12" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B16" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>83</v>
-      </c>
       <c r="D16" s="13" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="F16" s="6"/>
+        <v>94</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="194.25">
       <c r="A17" s="6" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="F17" s="6"/>
+        <v>99</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>100</v>
+      </c>
     </row>
-    <row r="18" spans="1:6" ht="205.5" customHeight="1">
+    <row r="18" spans="1:6" ht="243">
       <c r="A18" s="6" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="205.5" customHeight="1">
       <c r="A19" s="6" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="243">
       <c r="A20" s="6" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="178.5">
       <c r="A21" s="6" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="F21" s="6"/>
+        <v>123</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>124</v>
+      </c>
     </row>
-    <row r="22" spans="1:6" ht="113.25">
+    <row r="22" spans="1:6" ht="210.75">
       <c r="A22" s="6" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
+        <v>126</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>130</v>
+      </c>
     </row>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="24" spans="1:6" ht="64.5">
-      <c r="A24" s="12" t="s">
-        <v>118</v>
+    <row r="23" spans="1:6" ht="307.5">
+      <c r="A23" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="113.25">
+      <c r="A24" s="6" t="s">
+        <v>137</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
+        <v>138</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E24" s="14"/>
     </row>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="25" spans="1:6" ht="54" customHeight="1">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="1:6" ht="15.75">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="5"/>
+    </row>
     <row r="27" spans="1:6" ht="15.75" customHeight="1"/>
     <row r="28" spans="1:6" ht="15.75" customHeight="1"/>
     <row r="29" spans="1:6" ht="15.75" customHeight="1"/>
@@ -2441,8 +2708,17 @@
     <hyperlink ref="F10" r:id="rId9" location="consistent-navigation" xr:uid="{61432BEA-AFD2-4E9B-A153-619782D49F58}"/>
     <hyperlink ref="F13" r:id="rId10" xr:uid="{9D134B1A-4F6D-447C-97CA-2165353E4E66}"/>
     <hyperlink ref="F18" r:id="rId11" xr:uid="{43FEEA1C-9F19-44BE-AC03-C36B4EC3F43C}"/>
-    <hyperlink ref="F19" r:id="rId12" xr:uid="{6CEDF922-0E98-44C7-8CB3-CA5D7F6F7CF1}"/>
-    <hyperlink ref="F20" r:id="rId13" xr:uid="{D90F8BF8-4C36-40F5-96C1-2BCFAF65F3D4}"/>
+    <hyperlink ref="F20" r:id="rId12" xr:uid="{D90F8BF8-4C36-40F5-96C1-2BCFAF65F3D4}"/>
+    <hyperlink ref="F19" r:id="rId13" xr:uid="{06C557E6-EADC-433E-A9C1-A71E5FA3362C}"/>
+    <hyperlink ref="F11" r:id="rId14" location="link-purpose-in-context" xr:uid="{BE2FD37F-BC02-4B65-A0DE-5BA4A3876B0C}"/>
+    <hyperlink ref="F12" r:id="rId15" xr:uid="{23D8EEB5-6182-4B54-AD48-EF85E84E65D3}"/>
+    <hyperlink ref="F14" r:id="rId16" xr:uid="{2ED9684B-C15D-46C3-AC78-E8F5E6680C7D}"/>
+    <hyperlink ref="F15" r:id="rId17" location="close" xr:uid="{1FD9B639-F3CE-4877-8B08-161DA23905FD}"/>
+    <hyperlink ref="F16" r:id="rId18" location="close" xr:uid="{3156FC8B-1699-4DA0-870B-F311E9C03781}"/>
+    <hyperlink ref="F17" r:id="rId19" xr:uid="{099EAC60-A56D-4BA3-BD98-F213986B13E1}"/>
+    <hyperlink ref="F21" r:id="rId20" xr:uid="{598CB0BB-EF84-4B26-9C48-CC7D76FA54D5}"/>
+    <hyperlink ref="F23" r:id="rId21" xr:uid="{9BBA3A75-6840-4090-BF5B-90FB4579A4A0}"/>
+    <hyperlink ref="F22" r:id="rId22" xr:uid="{84311A4A-1784-4022-AE8C-F5147E8AD506}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
Added Accessibility-11 to the SEO-Template
</commit_message>
<xml_diff>
--- a/Template-SEO-audit.xlsx
+++ b/Template-SEO-audit.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25915"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicopatsch/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="944" documentId="11_05D6EA6CE7DA307BAFC13D42CE951501BDC39C52" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72D166D4-3F39-4315-AF35-AE16BFDE4520}"/>
+  <xr:revisionPtr revIDLastSave="991" documentId="11_05D6EA6CE7DA307BAFC13D42CE951501BDC39C52" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F3F872E-9957-4EB5-A719-80237043BF90}"/>
   <bookViews>
     <workbookView xWindow="940" yWindow="460" windowWidth="27860" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="145">
   <si>
     <t>Category</t>
   </si>
@@ -83,13 +83,13 @@
     <t>Accessibility-2</t>
   </si>
   <si>
-    <t>The page title is missing or not descriptive.</t>
+    <t>The page title is not descriptive.</t>
   </si>
   <si>
     <t>A descriptive title helps users understand a page's purpose or content. Without a proper title, many users (especially those using screen readers or other assistive technology) may have difficulty orienting themselves to the page.</t>
   </si>
   <si>
-    <t>Add titles to web pages that describe topic or purpose.</t>
+    <t>Add titles to web pages that describe topic or purpose. (Adding keywords here is most important for SEO, but do it in a natural way for best user experince.)</t>
   </si>
   <si>
     <r>
@@ -409,6 +409,42 @@
       </rPr>
       <t>&lt;/a</t>
     </r>
+  </si>
+  <si>
+    <t>Accessibility-11</t>
+  </si>
+  <si>
+    <t>Keyboard focus indicator was not visible.</t>
+  </si>
+  <si>
+    <t>Keyboard focus indicator helps anyone who relies on the keyboard to operate the page, by letting them visually determine the component on which keyboard operations will interact at any point in time.</t>
+  </si>
+  <si>
+    <t>It's always good to have a highlighted keyboard focus indicator, style it the way you like as long as it stands out from the surroundings.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Add the the focus pseudo-class likewise to your CSS:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>:focus {
+  outline: 2px solid black !important;
+}</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.w3.org/WAI/WCAG21/quickref/?showtechniques=247#focus-visible</t>
   </si>
   <si>
     <t>SEO-1</t>
@@ -802,9 +838,6 @@
   </si>
   <si>
     <t>Line number references are from the code "Indentation style changes in code (personal pref)" commit not from the original version of the code, for easier comparison with the amended version.</t>
-  </si>
-  <si>
-    <t>Simply put, the more quality links you have, the higher your authority, and therefore, the better your ranking is.</t>
   </si>
 </sst>
 </file>
@@ -921,7 +954,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -954,13 +987,16 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1177,10 +1213,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1001"/>
+  <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
@@ -1236,7 +1272,7 @@
       <c r="Z1" s="3"/>
     </row>
     <row r="2" spans="1:26" ht="113.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="14" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -1256,7 +1292,7 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="162">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="14" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -1277,7 +1313,7 @@
       <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:26" ht="275.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="14" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="6" t="s">
@@ -1421,7 +1457,7 @@
       <c r="D10" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="12" t="s">
         <v>60</v>
       </c>
       <c r="F10" s="5" t="s">
@@ -1449,17 +1485,17 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="162">
+    <row r="12" spans="1:26" ht="180" customHeight="1">
       <c r="A12" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="12" t="s">
         <v>70</v>
       </c>
       <c r="E12" s="6" t="s">
@@ -1468,16 +1504,15 @@
       <c r="F12" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="G12" s="6"/>
     </row>
-    <row r="13" spans="1:26" ht="275.25">
+    <row r="13" spans="1:26" ht="162">
       <c r="A13" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="12" t="s">
         <v>75</v>
       </c>
       <c r="D13" s="6" t="s">
@@ -1489,12 +1524,13 @@
       <c r="F13" s="5" t="s">
         <v>78</v>
       </c>
+      <c r="G13" s="6"/>
     </row>
-    <row r="14" spans="1:26" ht="96.75">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:26" ht="275.25">
+      <c r="A14" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="12" t="s">
         <v>80</v>
       </c>
       <c r="C14" s="6" t="s">
@@ -1509,13 +1545,12 @@
       <c r="F14" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="G14" s="11"/>
     </row>
-    <row r="15" spans="1:26" ht="146.25">
-      <c r="A15" s="12" t="s">
+    <row r="15" spans="1:26" ht="96.75">
+      <c r="A15" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="12" t="s">
         <v>86</v>
       </c>
       <c r="C15" s="6" t="s">
@@ -1530,48 +1565,49 @@
       <c r="F15" s="5" t="s">
         <v>90</v>
       </c>
+      <c r="G15" s="11"/>
     </row>
-    <row r="16" spans="1:26" ht="113.25">
-      <c r="A16" s="12" t="s">
+    <row r="16" spans="1:26" ht="146.25">
+      <c r="A16" s="15" t="s">
         <v>91</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>92</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="D16" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="D16" s="6" t="s">
         <v>94</v>
       </c>
+      <c r="E16" s="6" t="s">
+        <v>95</v>
+      </c>
       <c r="F16" s="5" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="194.25">
-      <c r="A17" s="6" t="s">
-        <v>95</v>
+    <row r="17" spans="1:6" ht="113.25">
+      <c r="A17" s="15" t="s">
+        <v>97</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="F17" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>100</v>
-      </c>
     </row>
-    <row r="18" spans="1:6" ht="243">
+    <row r="18" spans="1:6" ht="194.25">
       <c r="A18" s="6" t="s">
         <v>101</v>
       </c>
@@ -1581,7 +1617,7 @@
       <c r="C18" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="12" t="s">
         <v>104</v>
       </c>
       <c r="E18" s="6" t="s">
@@ -1591,7 +1627,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="205.5" customHeight="1">
+    <row r="19" spans="1:6" ht="243">
       <c r="A19" s="6" t="s">
         <v>107</v>
       </c>
@@ -1611,7 +1647,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="243">
+    <row r="20" spans="1:6" ht="205.5" customHeight="1">
       <c r="A20" s="6" t="s">
         <v>113</v>
       </c>
@@ -1631,7 +1667,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="178.5">
+    <row r="21" spans="1:6" ht="243">
       <c r="A21" s="6" t="s">
         <v>119</v>
       </c>
@@ -1641,7 +1677,7 @@
       <c r="C21" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="6" t="s">
         <v>122</v>
       </c>
       <c r="E21" s="6" t="s">
@@ -1651,17 +1687,17 @@
         <v>124</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="210.75">
+    <row r="22" spans="1:6" ht="178.5">
       <c r="A22" s="6" t="s">
         <v>125</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="12" t="s">
         <v>128</v>
       </c>
       <c r="E22" s="6" t="s">
@@ -1671,14 +1707,14 @@
         <v>130</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="307.5">
-      <c r="A23" s="6" t="s">
+    <row r="23" spans="1:6" ht="210.75">
+      <c r="A23" s="14" t="s">
         <v>131</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="12" t="s">
         <v>133</v>
       </c>
       <c r="D23" s="6" t="s">
@@ -1691,28 +1727,38 @@
         <v>136</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="113.25">
-      <c r="A24" s="6" t="s">
+    <row r="24" spans="1:6" ht="307.5">
+      <c r="A24" s="14" t="s">
         <v>137</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="C24" s="6"/>
+      <c r="C24" s="12" t="s">
+        <v>139</v>
+      </c>
       <c r="D24" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="E24" s="14"/>
+        <v>140</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>142</v>
+      </c>
     </row>
-    <row r="25" spans="1:6" ht="54" customHeight="1">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
+    <row r="25" spans="1:6" ht="113.25">
+      <c r="A25" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>144</v>
+      </c>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="5"/>
+      <c r="E25" s="13"/>
     </row>
-    <row r="26" spans="1:6" ht="15.75">
+    <row r="26" spans="1:6" ht="54" customHeight="1">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -1720,7 +1766,14 @@
       <c r="E26" s="6"/>
       <c r="F26" s="5"/>
     </row>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="27" spans="1:6" ht="15.75">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="5"/>
+    </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1"/>
     <row r="29" spans="1:6" ht="15.75" customHeight="1"/>
     <row r="30" spans="1:6" ht="15.75" customHeight="1"/>
@@ -2695,6 +2748,7 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
     <row r="1001" ht="15.75" customHeight="1"/>
+    <row r="1002" ht="15.75" customHeight="1"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" location="language-of-page" xr:uid="{BDC05546-EDF3-4630-92C7-EE1076FF788B}"/>
@@ -2706,19 +2760,20 @@
     <hyperlink ref="F3" r:id="rId7" location="sc2.4.2" xr:uid="{B37EBE60-CB4A-4274-AEAA-7F265BDC07CE}"/>
     <hyperlink ref="F9" r:id="rId8" location="contrast-minimum" xr:uid="{B7094FDD-1C54-49B5-81A5-957754EFEB60}"/>
     <hyperlink ref="F10" r:id="rId9" location="consistent-navigation" xr:uid="{61432BEA-AFD2-4E9B-A153-619782D49F58}"/>
-    <hyperlink ref="F13" r:id="rId10" xr:uid="{9D134B1A-4F6D-447C-97CA-2165353E4E66}"/>
-    <hyperlink ref="F18" r:id="rId11" xr:uid="{43FEEA1C-9F19-44BE-AC03-C36B4EC3F43C}"/>
-    <hyperlink ref="F20" r:id="rId12" xr:uid="{D90F8BF8-4C36-40F5-96C1-2BCFAF65F3D4}"/>
-    <hyperlink ref="F19" r:id="rId13" xr:uid="{06C557E6-EADC-433E-A9C1-A71E5FA3362C}"/>
+    <hyperlink ref="F14" r:id="rId10" xr:uid="{9D134B1A-4F6D-447C-97CA-2165353E4E66}"/>
+    <hyperlink ref="F19" r:id="rId11" xr:uid="{43FEEA1C-9F19-44BE-AC03-C36B4EC3F43C}"/>
+    <hyperlink ref="F21" r:id="rId12" xr:uid="{D90F8BF8-4C36-40F5-96C1-2BCFAF65F3D4}"/>
+    <hyperlink ref="F20" r:id="rId13" xr:uid="{06C557E6-EADC-433E-A9C1-A71E5FA3362C}"/>
     <hyperlink ref="F11" r:id="rId14" location="link-purpose-in-context" xr:uid="{BE2FD37F-BC02-4B65-A0DE-5BA4A3876B0C}"/>
-    <hyperlink ref="F12" r:id="rId15" xr:uid="{23D8EEB5-6182-4B54-AD48-EF85E84E65D3}"/>
-    <hyperlink ref="F14" r:id="rId16" xr:uid="{2ED9684B-C15D-46C3-AC78-E8F5E6680C7D}"/>
-    <hyperlink ref="F15" r:id="rId17" location="close" xr:uid="{1FD9B639-F3CE-4877-8B08-161DA23905FD}"/>
-    <hyperlink ref="F16" r:id="rId18" location="close" xr:uid="{3156FC8B-1699-4DA0-870B-F311E9C03781}"/>
-    <hyperlink ref="F17" r:id="rId19" xr:uid="{099EAC60-A56D-4BA3-BD98-F213986B13E1}"/>
-    <hyperlink ref="F21" r:id="rId20" xr:uid="{598CB0BB-EF84-4B26-9C48-CC7D76FA54D5}"/>
-    <hyperlink ref="F23" r:id="rId21" xr:uid="{9BBA3A75-6840-4090-BF5B-90FB4579A4A0}"/>
-    <hyperlink ref="F22" r:id="rId22" xr:uid="{84311A4A-1784-4022-AE8C-F5147E8AD506}"/>
+    <hyperlink ref="F13" r:id="rId15" xr:uid="{23D8EEB5-6182-4B54-AD48-EF85E84E65D3}"/>
+    <hyperlink ref="F15" r:id="rId16" xr:uid="{2ED9684B-C15D-46C3-AC78-E8F5E6680C7D}"/>
+    <hyperlink ref="F16" r:id="rId17" location="close" xr:uid="{1FD9B639-F3CE-4877-8B08-161DA23905FD}"/>
+    <hyperlink ref="F17" r:id="rId18" location="close" xr:uid="{3156FC8B-1699-4DA0-870B-F311E9C03781}"/>
+    <hyperlink ref="F18" r:id="rId19" xr:uid="{099EAC60-A56D-4BA3-BD98-F213986B13E1}"/>
+    <hyperlink ref="F22" r:id="rId20" xr:uid="{598CB0BB-EF84-4B26-9C48-CC7D76FA54D5}"/>
+    <hyperlink ref="F24" r:id="rId21" xr:uid="{9BBA3A75-6840-4090-BF5B-90FB4579A4A0}"/>
+    <hyperlink ref="F23" r:id="rId22" xr:uid="{84311A4A-1784-4022-AE8C-F5147E8AD506}"/>
+    <hyperlink ref="F12" r:id="rId23" location="focus-visible" xr:uid="{7D32ED94-2023-4963-9304-E3EAC4743829}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>